<commit_message>
add point_of_interest and establishment
</commit_message>
<xml_diff>
--- a/classification_matching/GOOGLE API BUSSINESS TYPE NAMES.xlsx
+++ b/classification_matching/GOOGLE API BUSSINESS TYPE NAMES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihongtan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9EBEDE6-ADD7-4407-B6C9-F409078455E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A12391-AE67-470F-8A20-533106EAC7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4100" yWindow="500" windowWidth="28800" windowHeight="16240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="190">
   <si>
     <t>GOOGLE API ALL BUSINESS TYPE</t>
   </si>
@@ -629,12 +629,15 @@
   <si>
     <t>zoo</t>
   </si>
+  <si>
+    <t>FOOD RETAI,FOOD SERVICE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -697,6 +700,18 @@
       <color theme="5"/>
       <name val="Batang"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Batang"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="-Apple-System"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -724,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -749,6 +764,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,10 +987,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A32" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -1290,7 +1310,7 @@
       </c>
       <c r="M11" t="str">
         <f>VLOOKUP(J11,A:E,2,TRUE)</f>
-        <v>FOOD RETAIL</v>
+        <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="36">
@@ -2007,9 +2027,9 @@
       <c r="K38" s="1">
         <v>1</v>
       </c>
-      <c r="M38" t="str">
+      <c r="M38">
         <f>VLOOKUP(J38,A:E,2,TRUE)</f>
-        <v>FOOD SERVICE</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="36">
@@ -2159,126 +2179,129 @@
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30.75">
+    <row r="44" spans="1:13" ht="15">
       <c r="A44" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B44" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>85</v>
-      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K44" s="1">
-        <v>7</v>
-      </c>
-      <c r="M44" t="str">
-        <f>VLOOKUP(J44,A:E,2,TRUE)</f>
-        <v>FOOD RETAIL</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="36">
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="1:13" ht="30.75">
       <c r="A45" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>54</v>
+        <v>120</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="13" t="s">
-        <v>55</v>
+      <c r="G45" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K45" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M45" t="str">
         <f>VLOOKUP(J45,A:E,2,TRUE)</f>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="24">
+    <row r="46" spans="1:13" ht="36">
       <c r="A46" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="13" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="K46" s="1">
         <v>1</v>
       </c>
-      <c r="M46">
+      <c r="M46" t="str">
         <f>VLOOKUP(J46,A:E,2,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="15">
+        <v>FOOD RETAIL</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="24">
       <c r="A47" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
+      <c r="G47" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="J47" s="1" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="K47" s="1">
         <v>1</v>
       </c>
-      <c r="M47" t="str">
+      <c r="M47">
         <f>VLOOKUP(J47,A:E,2,TRUE)</f>
-        <v>FOOD PRODUCTION AND PREPARATION</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15">
       <c r="A48" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
+      <c r="J48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K48" s="1">
+        <v>1</v>
+      </c>
+      <c r="M48" t="str">
+        <f>VLOOKUP(J48,A:E,2,TRUE)</f>
+        <v>FOOD PRODUCTION AND PREPARATION</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="15">
       <c r="A49" s="6" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -2288,321 +2311,312 @@
     </row>
     <row r="50" spans="1:7" ht="15">
       <c r="A50" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:7" ht="15.75">
+    <row r="51" spans="1:7" ht="15">
       <c r="A51" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75">
+      <c r="A52" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="8" t="s">
+      <c r="B52" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F52" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G52" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15">
-      <c r="A52" s="6" t="s">
+    <row r="53" spans="1:7" ht="15">
+      <c r="A53" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" s="10" t="s">
+      <c r="B53" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D53" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="7"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.75">
-      <c r="A53" s="6" t="s">
+      <c r="E53" s="11"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75">
+      <c r="A54" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="8" t="s">
+      <c r="B54" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D54" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F54" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G53" s="12" t="s">
+      <c r="G54" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="15">
-      <c r="A54" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:7" ht="15">
       <c r="A55" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>135</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="1:7" ht="48">
+    <row r="56" spans="1:7" ht="15">
       <c r="A56" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>138</v>
+        <v>80</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
-      <c r="G56" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="15">
+    </row>
+    <row r="57" spans="1:7" ht="48">
       <c r="A57" s="6" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
+      <c r="G57" s="13" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="15">
       <c r="A58" s="6" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>85</v>
+        <v>38</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="1:7" ht="36">
+    <row r="59" spans="1:7" ht="15">
       <c r="A59" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15">
+    </row>
+    <row r="60" spans="1:7" ht="36">
       <c r="A60" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>21</v>
+        <v>142</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
+      <c r="G60" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="61" spans="1:7" ht="15">
       <c r="A61" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:7" ht="15">
       <c r="A62" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
     </row>
-    <row r="63" spans="1:7" ht="24">
+    <row r="63" spans="1:7" ht="15">
       <c r="A63" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:7" ht="24">
+      <c r="A64" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B64" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C64" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D64" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E64" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F63" s="8" t="s">
+      <c r="F64" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G63" s="13" t="s">
+      <c r="G64" s="13" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="15">
-      <c r="A64" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:7" ht="15">
       <c r="A65" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:7" ht="15">
+      <c r="A66" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B66" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C66" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D66" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F65" s="8" t="s">
+      <c r="F66" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G66" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="60">
-      <c r="A66" s="7" t="s">
+    <row r="67" spans="1:7" ht="60">
+      <c r="A67" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B67" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C67" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D67" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="13" t="s">
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="13" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="36">
-      <c r="A67" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="36">
       <c r="A68" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="13" t="s">
@@ -2611,129 +2625,137 @@
     </row>
     <row r="69" spans="1:7" ht="15">
       <c r="A69" s="6" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
-    </row>
-    <row r="70" spans="1:7" ht="15">
+      <c r="G69" s="13"/>
+    </row>
+    <row r="70" spans="1:7" ht="36">
       <c r="A70" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
+        <v>152</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
+      <c r="G70" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="71" spans="1:7" ht="15">
       <c r="A71" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
+        <v>94</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="1:7" ht="24">
+    <row r="72" spans="1:7" ht="15">
       <c r="A72" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>156</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
     </row>
     <row r="73" spans="1:7" ht="15">
       <c r="A73" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
+        <v>154</v>
+      </c>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
     </row>
     <row r="74" spans="1:7" ht="24">
       <c r="A74" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="F74" s="10" t="s">
-        <v>160</v>
+        <v>13</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15">
       <c r="A75" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-    </row>
-    <row r="76" spans="1:7" ht="15">
+        <v>123</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="1:7" ht="24">
       <c r="A76" s="6" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="77" spans="1:7" ht="15">
       <c r="A77" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -2743,249 +2765,234 @@
     </row>
     <row r="78" spans="1:7" ht="15">
       <c r="A78" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
     </row>
     <row r="79" spans="1:7" ht="15">
       <c r="A79" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>157</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="1:7" ht="24">
+    <row r="80" spans="1:7" ht="15">
       <c r="A80" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B80" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="1:7" ht="15">
+      <c r="A81" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="10" t="s">
+      <c r="C81" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D80" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="F80" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="G80" s="13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="36">
-      <c r="A81" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="D81" s="7"/>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
-      <c r="G81" s="13" t="s">
+    </row>
+    <row r="82" spans="1:7" ht="24">
+      <c r="A82" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="36">
+      <c r="A83" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="13" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="15">
-      <c r="A82" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-    </row>
-    <row r="83" spans="1:7" ht="24">
-      <c r="A83" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G83" s="13" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15">
       <c r="A84" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:7" ht="15">
+    <row r="85" spans="1:7" ht="24">
       <c r="A85" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>172</v>
+        <v>76</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G85" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="86" spans="1:7" ht="15">
       <c r="A86" s="6" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" s="7"/>
-      <c r="D86" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
     </row>
-    <row r="87" spans="1:7" ht="24">
+    <row r="87" spans="1:7" ht="15">
       <c r="A87" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+    </row>
+    <row r="88" spans="1:7" ht="15">
+      <c r="A88" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+    </row>
+    <row r="89" spans="1:7" ht="24">
+      <c r="A89" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B87" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C87" s="8" t="s">
+      <c r="B89" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D89" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E89" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F87" s="8" t="s">
+      <c r="F89" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G87" s="13" t="s">
+      <c r="G89" s="13" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="24">
-      <c r="A88" s="6" t="s">
+    <row r="90" spans="1:7" ht="24">
+      <c r="A90" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B88" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C88" s="5" t="s">
+      <c r="B90" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D88" s="7"/>
-      <c r="E88" s="5" t="s">
+      <c r="D90" s="7"/>
+      <c r="E90" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F90" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G88" s="13" t="s">
+      <c r="G90" s="13" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="15">
-      <c r="A89" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-    </row>
-    <row r="90" spans="1:7" ht="15.75">
-      <c r="A90" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G90" s="12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15">
       <c r="A91" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
     </row>
     <row r="92" spans="1:7" ht="15.75">
       <c r="A92" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>11</v>
@@ -3006,117 +3013,156 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15.75">
+    <row r="93" spans="1:7" ht="15">
       <c r="A93" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+    </row>
+    <row r="94" spans="1:7" ht="15.75">
+      <c r="A94" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15.75">
+      <c r="A95" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C93" s="8" t="s">
+      <c r="B95" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D93" s="8" t="s">
+      <c r="D95" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E93" s="8" t="s">
+      <c r="E95" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F93" s="8" t="s">
+      <c r="F95" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G93" s="12" t="s">
+      <c r="G95" s="12" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="15">
-      <c r="A94" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-    </row>
-    <row r="95" spans="1:7" ht="24">
-      <c r="A95" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="G95" s="13" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15">
       <c r="A96" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="1:6" ht="15">
+    <row r="97" spans="1:7" ht="24">
       <c r="A97" s="6" t="s">
-        <v>188</v>
+        <v>27</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E97" s="7"/>
-      <c r="F97" s="7"/>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="7"/>
-      <c r="B98" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G97" s="13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15">
+      <c r="A98" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7"/>
+    <row r="99" spans="1:7" ht="15">
+      <c r="A99" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:7">
       <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
+      <c r="B100" s="4"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3125,10 +3171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EBE679-0237-40D7-B496-4CDAC14B8EDC}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3136,7 +3182,7 @@
     <col min="1" max="1" width="52.140625" customWidth="1"/>
     <col min="2" max="2" width="60" customWidth="1"/>
     <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
     <col min="5" max="5" width="42.85546875" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
     <col min="7" max="7" width="124.5703125" customWidth="1"/>
@@ -3776,356 +3822,350 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30.75">
+    <row r="33" spans="1:7" ht="15">
       <c r="A33" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>85</v>
-      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="36">
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7" ht="30.75">
       <c r="A34" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>54</v>
+        <v>120</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="24">
+      <c r="G34" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="36">
       <c r="A35" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="24">
       <c r="A36" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75">
+      <c r="G36" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15">
       <c r="A37" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75">
+      <c r="A38" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="8" t="s">
+      <c r="B38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D38" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="G38" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15">
-      <c r="A38" s="6" t="s">
+    <row r="39" spans="1:7" ht="15">
+      <c r="A39" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="10" t="s">
+      <c r="B39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75">
-      <c r="A39" s="6" t="s">
+      <c r="E39" s="11"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75">
+      <c r="A40" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="8" t="s">
+      <c r="B40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G39" s="12" t="s">
+      <c r="G40" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15">
-      <c r="A40" s="6" t="s">
+    <row r="41" spans="1:7" ht="15">
+      <c r="A41" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" ht="48">
-      <c r="A41" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15">
+    </row>
+    <row r="42" spans="1:7" ht="48">
       <c r="A42" s="6" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
+      <c r="G42" s="13" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="15">
       <c r="A43" s="6" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>85</v>
+        <v>38</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
     </row>
-    <row r="44" spans="1:7" ht="36">
+    <row r="44" spans="1:7" ht="15">
       <c r="A44" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15">
+    </row>
+    <row r="45" spans="1:7" ht="36">
       <c r="A45" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>21</v>
+        <v>142</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
+      <c r="G45" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="15">
       <c r="A46" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
     </row>
     <row r="47" spans="1:7" ht="15">
       <c r="A47" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:7" ht="24">
+    <row r="48" spans="1:7" ht="15">
       <c r="A48" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" ht="24">
+      <c r="A49" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B49" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C49" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F49" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G48" s="13" t="s">
+      <c r="G49" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15">
-      <c r="A49" s="6" t="s">
+    <row r="50" spans="1:7" ht="15">
+      <c r="A50" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F50" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="60">
-      <c r="A50" s="7" t="s">
+    <row r="51" spans="1:7" ht="60">
+      <c r="A51" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B51" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C51" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D51" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="13" t="s">
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="36">
-      <c r="A51" s="6" t="s">
+    <row r="52" spans="1:7" ht="36">
+      <c r="A52" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="15">
-      <c r="A52" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>11</v>
@@ -4138,269 +4178,257 @@
       </c>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
-    </row>
-    <row r="53" spans="1:7" ht="24">
+      <c r="G52" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15">
       <c r="A53" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G53" s="13" t="s">
-        <v>156</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="13"/>
     </row>
     <row r="54" spans="1:7" ht="15">
       <c r="A54" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:7" ht="24">
       <c r="A55" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>160</v>
+        <v>13</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15">
       <c r="A56" s="6" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-    </row>
-    <row r="57" spans="1:7" ht="15">
+        <v>53</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:7" ht="24">
       <c r="A57" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>46</v>
+        <v>7</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
+        <v>158</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="15">
       <c r="A58" s="6" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>157</v>
+        <v>38</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="1:7" ht="24">
+    <row r="59" spans="1:7" ht="15">
       <c r="A59" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:7" ht="15">
+      <c r="A60" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="36">
-      <c r="A60" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="13" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="61" spans="1:7" ht="24">
       <c r="A61" s="6" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>46</v>
+        <v>83</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>49</v>
+        <v>158</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>167</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="36">
       <c r="A62" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>21</v>
+        <v>169</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="1:7" ht="15">
+      <c r="G62" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="24">
       <c r="A63" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>172</v>
+        <v>76</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="15">
       <c r="A64" s="6" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:7" ht="24">
+    <row r="65" spans="1:7" ht="15">
       <c r="A65" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:7" ht="15">
+      <c r="A66" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:7" ht="24">
+      <c r="A67" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G65" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="24">
-      <c r="A66" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D66" s="7"/>
-      <c r="E66" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="G66" s="13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75">
-      <c r="A67" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>11</v>
@@ -4417,29 +4445,34 @@
       <c r="F67" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G67" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="15">
-      <c r="A68" s="6" t="s">
-        <v>181</v>
+      <c r="G67" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="24">
+      <c r="A68" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
+        <v>175</v>
+      </c>
+      <c r="D68" s="7"/>
+      <c r="E68" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="69" spans="1:7" ht="15.75">
-      <c r="A69" s="6" t="s">
-        <v>182</v>
+      <c r="A69" s="14" t="s">
+        <v>180</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>11</v>
@@ -4460,71 +4493,71 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15.75">
-      <c r="A70" s="6" t="s">
+    <row r="70" spans="1:7" ht="15">
+      <c r="A70" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:7" ht="15.75">
+      <c r="A71" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75">
+      <c r="A72" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="B70" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="8" t="s">
+      <c r="B72" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D72" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="8" t="s">
+      <c r="F72" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G70" s="12" t="s">
+      <c r="G72" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15">
-      <c r="A71" s="6" t="s">
+    <row r="73" spans="1:7" ht="15">
+      <c r="A73" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-    </row>
-    <row r="72" spans="1:7" ht="24">
-      <c r="A72" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="15">
-      <c r="A73" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>19</v>
@@ -4538,29 +4571,79 @@
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="7"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
+    <row r="74" spans="1:7" ht="24">
+      <c r="A74" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G74" s="13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15">
+      <c r="A75" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
+      <c r="A76" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test the code on frementle data
</commit_message>
<xml_diff>
--- a/classification_matching/GOOGLE API BUSSINESS TYPE NAMES.xlsx
+++ b/classification_matching/GOOGLE API BUSSINESS TYPE NAMES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihongtan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A12391-AE67-470F-8A20-533106EAC7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28FE2AB5-63CC-4A56-A2AD-715D66A8A5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4100" yWindow="500" windowWidth="28800" windowHeight="16240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="192">
   <si>
     <t>GOOGLE API ALL BUSINESS TYPE</t>
   </si>
@@ -630,7 +630,13 @@
     <t>zoo</t>
   </si>
   <si>
-    <t>FOOD RETAI,FOOD SERVICE</t>
+    <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">food </t>
+  </si>
+  <si>
+    <t>Food Production and Preparation</t>
   </si>
 </sst>
 </file>
@@ -713,7 +719,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -724,6 +730,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -739,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -768,7 +780,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3171,10 +3186,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EBE679-0237-40D7-B496-4CDAC14B8EDC}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A49" sqref="A29:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3189,7 +3204,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -3212,7 +3227,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -3235,7 +3250,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="45.75">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -3254,7 +3269,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="36">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3273,7 +3288,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="36">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3292,7 +3307,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3311,7 +3326,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="24">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -3334,7 +3349,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="24">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -3357,7 +3372,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="36">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -3376,7 +3391,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="36">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -3395,7 +3410,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -3418,7 +3433,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -3441,7 +3456,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="36">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -3460,7 +3475,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="16" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -3476,7 +3491,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="15">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="16" t="s">
         <v>79</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -3490,7 +3505,7 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="15">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="16" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3509,7 +3524,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="16" t="s">
         <v>87</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -3532,7 +3547,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="16" t="s">
         <v>89</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -3548,7 +3563,7 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="15">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="16" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -3566,7 +3581,7 @@
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="36">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="16" t="s">
         <v>96</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3585,7 +3600,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="24">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="16" t="s">
         <v>78</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -3604,7 +3619,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="36">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="16" t="s">
         <v>102</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -3623,7 +3638,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="36">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="16" t="s">
         <v>101</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -3642,7 +3657,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -3665,7 +3680,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="16" t="s">
         <v>108</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -3688,7 +3703,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="36">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="16" t="s">
         <v>110</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -3707,7 +3722,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="36">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="16" t="s">
         <v>112</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3726,7 +3741,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="36">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="16" t="s">
         <v>109</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -3745,7 +3760,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="16" t="s">
         <v>114</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -3763,7 +3778,7 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:7" ht="15">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="16" t="s">
         <v>117</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -3781,7 +3796,7 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:7" ht="24">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="16" t="s">
         <v>119</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -3804,7 +3819,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="36">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="16" t="s">
         <v>107</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -3823,7 +3838,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3836,7 +3851,7 @@
       <c r="G33" s="13"/>
     </row>
     <row r="34" spans="1:7" ht="30.75">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="16" t="s">
         <v>120</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -3855,7 +3870,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="36">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="16" t="s">
         <v>103</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -3874,7 +3889,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="24">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="16" t="s">
         <v>124</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -3893,7 +3908,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="16" t="s">
         <v>128</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -3909,7 +3924,7 @@
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:7" ht="15.75">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="16" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="8" t="s">
@@ -3932,7 +3947,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="16" t="s">
         <v>105</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -3948,7 +3963,7 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:7" ht="15.75">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="16" t="s">
         <v>132</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -3971,7 +3986,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="15">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="16" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -3987,7 +4002,7 @@
       <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:7" ht="48">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="16" t="s">
         <v>97</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -4006,7 +4021,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="15">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="16" t="s">
         <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -4022,7 +4037,7 @@
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:7" ht="15">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -4038,7 +4053,7 @@
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:7" ht="36">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="16" t="s">
         <v>142</v>
       </c>
       <c r="B45" s="8" t="s">
@@ -4057,7 +4072,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="16" t="s">
         <v>116</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -4073,7 +4088,7 @@
       <c r="F46" s="7"/>
     </row>
     <row r="47" spans="1:7" ht="15">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="16" t="s">
         <v>143</v>
       </c>
       <c r="B47" s="7"/>
@@ -4083,7 +4098,7 @@
       <c r="F47" s="7"/>
     </row>
     <row r="48" spans="1:7" ht="15">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="16" t="s">
         <v>144</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -4099,7 +4114,7 @@
       <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:7" ht="24">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="16" t="s">
         <v>145</v>
       </c>
       <c r="B49" s="8" t="s">
@@ -4635,15 +4650,16 @@
       <c r="F77" s="7"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
+      <c r="A78" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B78" t="s">
+        <v>191</v>
+      </c>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4651,26 +4667,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7219cb9b-9341-4b3b-a534-b87b88f60fe7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b0dc143a-c2fc-4156-aa7e-afa165885dad" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010082FA515920280A43BF703992ADDE5548" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75712c46411baca1e39ca86bd87e16fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b0dc143a-c2fc-4156-aa7e-afa165885dad" xmlns:ns3="7219cb9b-9341-4b3b-a534-b87b88f60fe7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1b648303ec20ccccb0d0becfb8e50d4" ns2:_="" ns3:_="">
     <xsd:import namespace="b0dc143a-c2fc-4156-aa7e-afa165885dad"/>
@@ -4887,8 +4883,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7219cb9b-9341-4b3b-a534-b87b88f60fe7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b0dc143a-c2fc-4156-aa7e-afa165885dad" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ADE671F-0529-4E8A-8FB0-A73F044F3567}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24D0452-19E6-4F01-835E-EDFFD925A1F6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4896,5 +4912,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24D0452-19E6-4F01-835E-EDFFD925A1F6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ADE671F-0529-4E8A-8FB0-A73F044F3567}"/>
 </file>
</xml_diff>